<commit_message>
Updates to bldgs/BCEU to fix python export issue and updated calibration doc
</commit_message>
<xml_diff>
--- a/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
+++ b/InputData/bldgs/BCEU/BAU Components Energy Use.xlsx
@@ -49658,100 +49658,100 @@
         </is>
       </c>
       <c r="J4" s="105" t="n">
-        <v>17288207961473.84</v>
+        <v>38034840244178.23</v>
       </c>
       <c r="K4" s="105" t="n">
-        <v>17278896582034.63</v>
+        <v>38122150486405.09</v>
       </c>
       <c r="L4" s="105" t="n">
-        <v>17270569875980.64</v>
+        <v>38185811448952.49</v>
       </c>
       <c r="M4" s="105" t="n">
-        <v>17259445471853.63</v>
+        <v>38210055922994.02</v>
       </c>
       <c r="N4" s="105" t="n">
-        <v>17252231643986.55</v>
+        <v>38218006563838.13</v>
       </c>
       <c r="O4" s="105" t="n">
-        <v>17255577410388.12</v>
+        <v>38208223115967.85</v>
       </c>
       <c r="P4" s="105" t="n">
-        <v>17272860489999.26</v>
+        <v>38191155026982.61</v>
       </c>
       <c r="Q4" s="105" t="n">
-        <v>17308386166096.59</v>
+        <v>38178964800693.44</v>
       </c>
       <c r="R4" s="105" t="n">
-        <v>17362272871599.13</v>
+        <v>38180762887158.05</v>
       </c>
       <c r="S4" s="105" t="n">
-        <v>17432314222230.78</v>
+        <v>38164043766564.98</v>
       </c>
       <c r="T4" s="105" t="n">
-        <v>17514174146728.25</v>
+        <v>38163668727231.16</v>
       </c>
       <c r="U4" s="105" t="n">
-        <v>17607863688800.86</v>
+        <v>38151446602023.98</v>
       </c>
       <c r="V4" s="105" t="n">
-        <v>17714012861631.05</v>
+        <v>38156642337137.23</v>
       </c>
       <c r="W4" s="105" t="n">
-        <v>17829786059034.79</v>
+        <v>38171722114094.51</v>
       </c>
       <c r="X4" s="105" t="n">
-        <v>17950406478555.66</v>
+        <v>38193904450133.29</v>
       </c>
       <c r="Y4" s="105" t="n">
-        <v>18077934083164.29</v>
+        <v>38250197384210.84</v>
       </c>
       <c r="Z4" s="105" t="n">
-        <v>18211341399358.73</v>
+        <v>38316099013471.23</v>
       </c>
       <c r="AA4" s="105" t="n">
-        <v>18351219643564.64</v>
+        <v>38428932683765.96</v>
       </c>
       <c r="AB4" s="105" t="n">
-        <v>18493165161922.13</v>
+        <v>38562327171100.45</v>
       </c>
       <c r="AC4" s="105" t="n">
-        <v>18634477030379.94</v>
+        <v>38714069881515.87</v>
       </c>
       <c r="AD4" s="105" t="n">
-        <v>18775167003771.56</v>
+        <v>38878863249974.98</v>
       </c>
       <c r="AE4" s="105" t="n">
-        <v>18914361613666.7</v>
+        <v>39065953269048.34</v>
       </c>
       <c r="AF4" s="105" t="n">
-        <v>19041450193765.03</v>
+        <v>39168925126596.66</v>
       </c>
       <c r="AG4" s="105" t="n">
-        <v>19167936097934.74</v>
+        <v>39274717624494.91</v>
       </c>
       <c r="AH4" s="105" t="n">
-        <v>19294420461203.48</v>
+        <v>39396011305801.26</v>
       </c>
       <c r="AI4" s="105" t="n">
-        <v>19420596320623.46</v>
+        <v>39520005257183.43</v>
       </c>
       <c r="AJ4" s="105" t="n">
-        <v>19547514925914.11</v>
+        <v>39652798856246.66</v>
       </c>
       <c r="AK4" s="105" t="n">
-        <v>19674836168172.98</v>
+        <v>39777276884326.42</v>
       </c>
       <c r="AL4" s="105" t="n">
-        <v>19803621638582</v>
+        <v>39904044611081.12</v>
       </c>
       <c r="AM4" s="105" t="n">
-        <v>19934496588446.38</v>
+        <v>40035231110406.28</v>
       </c>
       <c r="AN4" s="105" t="n">
-        <v>20067148264214.06</v>
+        <v>40170998076303.33</v>
       </c>
       <c r="AO4" s="105" t="n">
-        <v>20201293989281.95</v>
+        <v>40311602158951.76</v>
       </c>
     </row>
     <row r="5">
@@ -49869,100 +49869,100 @@
         </is>
       </c>
       <c r="J6" s="105" t="n">
-        <v>14414108903818.04</v>
+        <v>57525354469575.77</v>
       </c>
       <c r="K6" s="105" t="n">
-        <v>14504557267289.01</v>
+        <v>57614107674374.98</v>
       </c>
       <c r="L6" s="105" t="n">
-        <v>14599762277810.72</v>
+        <v>57679342034514.18</v>
       </c>
       <c r="M6" s="105" t="n">
-        <v>14694271355187.56</v>
+        <v>57690944543144.89</v>
       </c>
       <c r="N6" s="105" t="n">
-        <v>14790878708581.62</v>
+        <v>57675178881220.66</v>
       </c>
       <c r="O6" s="105" t="n">
-        <v>14892255760367.05</v>
+        <v>57635385593521.73</v>
       </c>
       <c r="P6" s="105" t="n">
-        <v>14998880876795.84</v>
+        <v>57590331343893.02</v>
       </c>
       <c r="Q6" s="105" t="n">
-        <v>15114885668489.68</v>
+        <v>57576974856354.38</v>
       </c>
       <c r="R6" s="105" t="n">
-        <v>15238587827887.84</v>
+        <v>57619107255086.85</v>
       </c>
       <c r="S6" s="105" t="n">
-        <v>15364027738763.4</v>
+        <v>57651888475416.22</v>
       </c>
       <c r="T6" s="105" t="n">
-        <v>15489080179906.57</v>
+        <v>57739784510091.62</v>
       </c>
       <c r="U6" s="105" t="n">
-        <v>15614560951615.01</v>
+        <v>57831920980606.51</v>
       </c>
       <c r="V6" s="105" t="n">
-        <v>15740680987347.2</v>
+        <v>57972144664112.52</v>
       </c>
       <c r="W6" s="105" t="n">
-        <v>15864282235547.63</v>
+        <v>58146276268731.36</v>
       </c>
       <c r="X6" s="105" t="n">
-        <v>15983886499556.45</v>
+        <v>58336563441827.06</v>
       </c>
       <c r="Y6" s="105" t="n">
-        <v>16107239931243.63</v>
+        <v>58575163883998.6</v>
       </c>
       <c r="Z6" s="105" t="n">
-        <v>16234016131046.76</v>
+        <v>58806480341637.41</v>
       </c>
       <c r="AA6" s="105" t="n">
-        <v>16365451831652.03</v>
+        <v>59109245669991.47</v>
       </c>
       <c r="AB6" s="105" t="n">
-        <v>16497606319706.33</v>
+        <v>59430759846532.81</v>
       </c>
       <c r="AC6" s="105" t="n">
-        <v>16629186521133.24</v>
+        <v>59756962051751.39</v>
       </c>
       <c r="AD6" s="105" t="n">
-        <v>16760892934697</v>
+        <v>60097238234171.22</v>
       </c>
       <c r="AE6" s="105" t="n">
-        <v>16891422593085</v>
+        <v>60468864892592.73</v>
       </c>
       <c r="AF6" s="105" t="n">
-        <v>16998753432451.8</v>
+        <v>60636922572941.8</v>
       </c>
       <c r="AG6" s="105" t="n">
-        <v>17105194476191.08</v>
+        <v>60802440277962.16</v>
       </c>
       <c r="AH6" s="105" t="n">
-        <v>17213528057661.44</v>
+        <v>61002169507944.09</v>
       </c>
       <c r="AI6" s="105" t="n">
-        <v>17323188181209.07</v>
+        <v>61219368584627.94</v>
       </c>
       <c r="AJ6" s="105" t="n">
-        <v>17435316690381.91</v>
+        <v>61475009805463.13</v>
       </c>
       <c r="AK6" s="105" t="n">
-        <v>17547654573222.37</v>
+        <v>61726810712570.43</v>
       </c>
       <c r="AL6" s="105" t="n">
-        <v>17661281905234.93</v>
+        <v>61986217146117.5</v>
       </c>
       <c r="AM6" s="105" t="n">
-        <v>17775792429044.64</v>
+        <v>62245484767178.63</v>
       </c>
       <c r="AN6" s="105" t="n">
-        <v>17891510366330.35</v>
+        <v>62496069009319.1</v>
       </c>
       <c r="AO6" s="105" t="n">
-        <v>18008735045303.26</v>
+        <v>62732667996920.9</v>
       </c>
     </row>
     <row r="7">
@@ -49977,100 +49977,100 @@
         </is>
       </c>
       <c r="J7" s="105" t="n">
-        <v>123250554775.973</v>
+        <v>5809108701386.697</v>
       </c>
       <c r="K7" s="105" t="n">
-        <v>121294448054.9675</v>
+        <v>5795106800135.362</v>
       </c>
       <c r="L7" s="105" t="n">
-        <v>119911269554.5207</v>
+        <v>5776507520198.192</v>
       </c>
       <c r="M7" s="105" t="n">
-        <v>118956465164.6592</v>
+        <v>5750018136897.318</v>
       </c>
       <c r="N7" s="105" t="n">
-        <v>118408180120.9932</v>
+        <v>5715422209082.903</v>
       </c>
       <c r="O7" s="105" t="n">
-        <v>118234786144.7561</v>
+        <v>5670848830904.343</v>
       </c>
       <c r="P7" s="105" t="n">
-        <v>118304078842.4644</v>
+        <v>5613918650014.564</v>
       </c>
       <c r="Q7" s="105" t="n">
-        <v>118596810702.1353</v>
+        <v>5544680819321.188</v>
       </c>
       <c r="R7" s="105" t="n">
-        <v>119071616831.286</v>
+        <v>5459683481913.548</v>
       </c>
       <c r="S7" s="105" t="n">
-        <v>119602968975.6994</v>
+        <v>5346762397170.606</v>
       </c>
       <c r="T7" s="105" t="n">
-        <v>120199850013.0476</v>
+        <v>5209617967003.282</v>
       </c>
       <c r="U7" s="105" t="n">
-        <v>120805185570.2927</v>
+        <v>5041540949527.341</v>
       </c>
       <c r="V7" s="105" t="n">
-        <v>121439908183.6804</v>
+        <v>4849167696797.911</v>
       </c>
       <c r="W7" s="105" t="n">
-        <v>122101588259.7885</v>
+        <v>4636920059144.704</v>
       </c>
       <c r="X7" s="105" t="n">
-        <v>122711282447.958</v>
+        <v>4406582100599.357</v>
       </c>
       <c r="Y7" s="105" t="n">
-        <v>123366210988.7159</v>
+        <v>4163288604796.895</v>
       </c>
       <c r="Z7" s="105" t="n">
-        <v>124006728279.3633</v>
+        <v>3906134068535.528</v>
       </c>
       <c r="AA7" s="105" t="n">
-        <v>124700319553.3777</v>
+        <v>3646270131408.625</v>
       </c>
       <c r="AB7" s="105" t="n">
-        <v>125392788302.5012</v>
+        <v>3382922970077.043</v>
       </c>
       <c r="AC7" s="105" t="n">
-        <v>126048492119.1729</v>
+        <v>3116854487710.78</v>
       </c>
       <c r="AD7" s="105" t="n">
-        <v>126728908933.4799</v>
+        <v>2851603829198.63</v>
       </c>
       <c r="AE7" s="105" t="n">
-        <v>127397256643.5693</v>
+        <v>2589939592870.796</v>
       </c>
       <c r="AF7" s="105" t="n">
-        <v>128092216288.536</v>
+        <v>2322863763620.604</v>
       </c>
       <c r="AG7" s="105" t="n">
-        <v>128745461972.2211</v>
+        <v>2064961925844.683</v>
       </c>
       <c r="AH7" s="105" t="n">
-        <v>129430757851.2287</v>
+        <v>1819352601588.479</v>
       </c>
       <c r="AI7" s="105" t="n">
-        <v>130115194601.12</v>
+        <v>1586873600535.047</v>
       </c>
       <c r="AJ7" s="105" t="n">
-        <v>130836332977.6488</v>
+        <v>1370386626337.891</v>
       </c>
       <c r="AK7" s="105" t="n">
-        <v>131521867003.6595</v>
+        <v>1171209170341.764</v>
       </c>
       <c r="AL7" s="105" t="n">
-        <v>132208154564.9921</v>
+        <v>991990341776.9606</v>
       </c>
       <c r="AM7" s="105" t="n">
-        <v>132894673797.7364</v>
+        <v>833755339335.3734</v>
       </c>
       <c r="AN7" s="105" t="n">
-        <v>133582959946.4173</v>
+        <v>696366126531.4026</v>
       </c>
       <c r="AO7" s="105" t="n">
-        <v>134274731220.2286</v>
+        <v>578994319161.5814</v>
       </c>
     </row>
     <row r="8">
@@ -50188,100 +50188,100 @@
         </is>
       </c>
       <c r="J9" s="105" t="n">
-        <v>3018439436380.831</v>
+        <v>9999824341374.98</v>
       </c>
       <c r="K9" s="105" t="n">
-        <v>3045506913063.016</v>
+        <v>9980247499422.994</v>
       </c>
       <c r="L9" s="105" t="n">
-        <v>3073376798226.763</v>
+        <v>9955258984691.482</v>
       </c>
       <c r="M9" s="105" t="n">
-        <v>3098927785305.183</v>
+        <v>9919766259612.26</v>
       </c>
       <c r="N9" s="105" t="n">
-        <v>3123928165816.791</v>
+        <v>9880121115516.891</v>
       </c>
       <c r="O9" s="105" t="n">
-        <v>3150036094746.871</v>
+        <v>9837459029467.998</v>
       </c>
       <c r="P9" s="105" t="n">
-        <v>3174967009231.748</v>
+        <v>9790480201557.172</v>
       </c>
       <c r="Q9" s="105" t="n">
-        <v>3200280316691.819</v>
+        <v>9746954552606.465</v>
       </c>
       <c r="R9" s="105" t="n">
-        <v>3226627151841.605</v>
+        <v>9707901087282.166</v>
       </c>
       <c r="S9" s="105" t="n">
-        <v>3250927926394.331</v>
+        <v>9663151725580.273</v>
       </c>
       <c r="T9" s="105" t="n">
-        <v>3275196063190.953</v>
+        <v>9623429963292.986</v>
       </c>
       <c r="U9" s="105" t="n">
-        <v>3297667205898.727</v>
+        <v>9578647397956.514</v>
       </c>
       <c r="V9" s="105" t="n">
-        <v>3319860239597.674</v>
+        <v>9537737749672.146</v>
       </c>
       <c r="W9" s="105" t="n">
-        <v>3342456929548.913</v>
+        <v>9504008271989.459</v>
       </c>
       <c r="X9" s="105" t="n">
-        <v>3362444943217.311</v>
+        <v>9471327440004.174</v>
       </c>
       <c r="Y9" s="105" t="n">
-        <v>3383356011829.254</v>
+        <v>9449407475763.877</v>
       </c>
       <c r="Z9" s="105" t="n">
-        <v>3402792842350.137</v>
+        <v>9432987115919.277</v>
       </c>
       <c r="AA9" s="105" t="n">
-        <v>3423694801102.421</v>
+        <v>9436208427658.812</v>
       </c>
       <c r="AB9" s="105" t="n">
-        <v>3444309167284.744</v>
+        <v>9452988079974.242</v>
       </c>
       <c r="AC9" s="105" t="n">
-        <v>3463227889500.59</v>
+        <v>9477482159277.09</v>
       </c>
       <c r="AD9" s="105" t="n">
-        <v>3483100310886.622</v>
+        <v>9510272239978.025</v>
       </c>
       <c r="AE9" s="105" t="n">
-        <v>3502419726688.582</v>
+        <v>9549412321267.697</v>
       </c>
       <c r="AF9" s="105" t="n">
-        <v>3519435571039.064</v>
+        <v>9575233906176.713</v>
       </c>
       <c r="AG9" s="105" t="n">
-        <v>3534703824929.354</v>
+        <v>9596994730409.035</v>
       </c>
       <c r="AH9" s="105" t="n">
-        <v>3551161584050.046</v>
+        <v>9618757404823.264</v>
       </c>
       <c r="AI9" s="105" t="n">
-        <v>3567401268410.946</v>
+        <v>9633915213437.279</v>
       </c>
       <c r="AJ9" s="105" t="n">
-        <v>3584952295137.564</v>
+        <v>9646355620026.131</v>
       </c>
       <c r="AK9" s="105" t="n">
-        <v>3600881523196.844</v>
+        <v>9649843270030.379</v>
       </c>
       <c r="AL9" s="105" t="n">
-        <v>3616689289277.442</v>
+        <v>9651166893471.473</v>
       </c>
       <c r="AM9" s="105" t="n">
-        <v>3632406953280.965</v>
+        <v>9652511775316.693</v>
       </c>
       <c r="AN9" s="105" t="n">
-        <v>3648068393521.221</v>
+        <v>9654011530418.453</v>
       </c>
       <c r="AO9" s="105" t="n">
-        <v>3663701546166.395</v>
+        <v>9655784194619.887</v>
       </c>
     </row>
     <row r="10">
@@ -50291,100 +50291,100 @@
         </is>
       </c>
       <c r="J10" s="93" t="n">
-        <v>114474375190.9566</v>
+        <v>784004068727.6968</v>
       </c>
       <c r="K10" s="93" t="n">
-        <v>114719948250.3018</v>
+        <v>783328009047.8948</v>
       </c>
       <c r="L10" s="93" t="n">
-        <v>115028136976.2639</v>
+        <v>782097934214.6171</v>
       </c>
       <c r="M10" s="93" t="n">
-        <v>115286931032.6444</v>
+        <v>779863462301.2625</v>
       </c>
       <c r="N10" s="93" t="n">
-        <v>115560065398.1628</v>
+        <v>776708739053.3181</v>
       </c>
       <c r="O10" s="93" t="n">
-        <v>115914412560.6918</v>
+        <v>772312244906.76</v>
       </c>
       <c r="P10" s="93" t="n">
-        <v>116239099798.9823</v>
+        <v>766130454977.696</v>
       </c>
       <c r="Q10" s="93" t="n">
-        <v>116562150993.3552</v>
+        <v>758158803759.0719</v>
       </c>
       <c r="R10" s="93" t="n">
-        <v>116912686489.7238</v>
+        <v>747807046552.1301</v>
       </c>
       <c r="S10" s="93" t="n">
-        <v>117200074605.1664</v>
+        <v>733683579276.5841</v>
       </c>
       <c r="T10" s="93" t="n">
-        <v>117500718475.1926</v>
+        <v>716329242605.9849</v>
       </c>
       <c r="U10" s="93" t="n">
-        <v>117748860430.6811</v>
+        <v>694907342497.7031</v>
       </c>
       <c r="V10" s="93" t="n">
-        <v>117994516167.4063</v>
+        <v>670353605052.243</v>
       </c>
       <c r="W10" s="93" t="n">
-        <v>118270999376.6042</v>
+        <v>643409564174.3796</v>
       </c>
       <c r="X10" s="93" t="n">
-        <v>118480466111.5032</v>
+        <v>614089414355.2697</v>
       </c>
       <c r="Y10" s="93" t="n">
-        <v>118740099451.6927</v>
+        <v>583146244375.4017</v>
       </c>
       <c r="Z10" s="93" t="n">
-        <v>118961450972.5707</v>
+        <v>550437713683.1467</v>
       </c>
       <c r="AA10" s="93" t="n">
-        <v>119247059412.2659</v>
+        <v>517156269300.7151</v>
       </c>
       <c r="AB10" s="93" t="n">
-        <v>119533241431.4017</v>
+        <v>483247762712.5033</v>
       </c>
       <c r="AC10" s="93" t="n">
-        <v>119770032535.1035</v>
+        <v>448817543258.5192</v>
       </c>
       <c r="AD10" s="93" t="n">
-        <v>120051417251.4579</v>
+        <v>414469606989.2194</v>
       </c>
       <c r="AE10" s="93" t="n">
-        <v>120331103847.5345</v>
+        <v>380688576936.8724</v>
       </c>
       <c r="AF10" s="93" t="n">
-        <v>120915709775.2563</v>
+        <v>347416892135.4872</v>
       </c>
       <c r="AG10" s="93" t="n">
-        <v>121440274501.3064</v>
+        <v>315629986267.3223</v>
       </c>
       <c r="AH10" s="93" t="n">
-        <v>122005706538.6944</v>
+        <v>285970119904.7526</v>
       </c>
       <c r="AI10" s="93" t="n">
-        <v>122563646276.868</v>
+        <v>258657970692.6342</v>
       </c>
       <c r="AJ10" s="93" t="n">
-        <v>123166639231.5897</v>
+        <v>234115688176.1829</v>
       </c>
       <c r="AK10" s="93" t="n">
-        <v>123713912758.2908</v>
+        <v>212365897083.6626</v>
       </c>
       <c r="AL10" s="93" t="n">
-        <v>124257013268.8742</v>
+        <v>193637836918.6214</v>
       </c>
       <c r="AM10" s="93" t="n">
-        <v>124797018181.7739</v>
+        <v>177936168081.1871</v>
       </c>
       <c r="AN10" s="93" t="n">
-        <v>125335091439.4111</v>
+        <v>165129940788.9165</v>
       </c>
       <c r="AO10" s="93" t="n">
-        <v>125872192832.507</v>
+        <v>154992845469.566</v>
       </c>
     </row>
     <row r="11">
@@ -50502,100 +50502,100 @@
         </is>
       </c>
       <c r="J12" s="105" t="n">
-        <v>2333258176944.205</v>
+        <v>6041889132056.472</v>
       </c>
       <c r="K12" s="105" t="n">
-        <v>2331331158017.752</v>
+        <v>6053034108480.291</v>
       </c>
       <c r="L12" s="105" t="n">
-        <v>2333518561576.784</v>
+        <v>6066482573597.639</v>
       </c>
       <c r="M12" s="105" t="n">
-        <v>2337557263822.965</v>
+        <v>6078623065222.982</v>
       </c>
       <c r="N12" s="105" t="n">
-        <v>2344199711734.208</v>
+        <v>6091858827416.873</v>
       </c>
       <c r="O12" s="105" t="n">
-        <v>2354060560552.396</v>
+        <v>6106483444511.795</v>
       </c>
       <c r="P12" s="105" t="n">
-        <v>2365429051259.618</v>
+        <v>6121255606864.683</v>
       </c>
       <c r="Q12" s="105" t="n">
-        <v>2379035107025.127</v>
+        <v>6139964536584.008</v>
       </c>
       <c r="R12" s="105" t="n">
-        <v>2394843216470.955</v>
+        <v>6163050264438.884</v>
       </c>
       <c r="S12" s="105" t="n">
-        <v>2410520831677.257</v>
+        <v>6183516541756.874</v>
       </c>
       <c r="T12" s="105" t="n">
-        <v>2426825588105.307</v>
+        <v>6207273851612.872</v>
       </c>
       <c r="U12" s="105" t="n">
-        <v>2442576183987.971</v>
+        <v>6228384744760.081</v>
       </c>
       <c r="V12" s="105" t="n">
-        <v>2458498234983.83</v>
+        <v>6250664990987.987</v>
       </c>
       <c r="W12" s="105" t="n">
-        <v>2474741364642.32</v>
+        <v>6274253796045.679</v>
       </c>
       <c r="X12" s="105" t="n">
-        <v>2489423764164.794</v>
+        <v>6294533547019.074</v>
       </c>
       <c r="Y12" s="105" t="n">
-        <v>2504818133415.796</v>
+        <v>6315665307144.612</v>
       </c>
       <c r="Z12" s="105" t="n">
-        <v>2519512493144.951</v>
+        <v>6331917026367.375</v>
       </c>
       <c r="AA12" s="105" t="n">
-        <v>2535217966709.433</v>
+        <v>6350433339256.21</v>
       </c>
       <c r="AB12" s="105" t="n">
-        <v>2550763112202.337</v>
+        <v>6366534155891.358</v>
       </c>
       <c r="AC12" s="105" t="n">
-        <v>2565309853627.783</v>
+        <v>6378305948307.742</v>
       </c>
       <c r="AD12" s="105" t="n">
-        <v>2580391920931.478</v>
+        <v>6389233321551.088</v>
       </c>
       <c r="AE12" s="105" t="n">
-        <v>2595091084234.612</v>
+        <v>6401080216909.914</v>
       </c>
       <c r="AF12" s="105" t="n">
-        <v>2608619497235.197</v>
+        <v>6401367102023.573</v>
       </c>
       <c r="AG12" s="105" t="n">
-        <v>2621108633091.339</v>
+        <v>6401002186899.102</v>
       </c>
       <c r="AH12" s="105" t="n">
-        <v>2634334542735.563</v>
+        <v>6405356993847.726</v>
       </c>
       <c r="AI12" s="105" t="n">
-        <v>2647476045551.269</v>
+        <v>6412729088167.57</v>
       </c>
       <c r="AJ12" s="105" t="n">
-        <v>2661448343265.092</v>
+        <v>6426101746137.92</v>
       </c>
       <c r="AK12" s="105" t="n">
-        <v>2674499965643.003</v>
+        <v>6440426838822.009</v>
       </c>
       <c r="AL12" s="105" t="n">
-        <v>2687527044949.619</v>
+        <v>6457581852987.034</v>
       </c>
       <c r="AM12" s="105" t="n">
-        <v>2700534366859.004</v>
+        <v>6476931052509.041</v>
       </c>
       <c r="AN12" s="105" t="n">
-        <v>2713554075950.199</v>
+        <v>6497548458396.054</v>
       </c>
       <c r="AO12" s="105" t="n">
-        <v>2726614646659.94</v>
+        <v>6518780712785.461</v>
       </c>
     </row>
     <row r="13">
@@ -55498,100 +55498,100 @@
         </is>
       </c>
       <c r="J69" s="105" t="n">
-        <v>5610080729219.988</v>
+        <v>12342431602415.45</v>
       </c>
       <c r="K69" s="105" t="n">
-        <v>5607059155759.581</v>
+        <v>12370764065124.84</v>
       </c>
       <c r="L69" s="105" t="n">
-        <v>5604357112073.186</v>
+        <v>12391422258269.35</v>
       </c>
       <c r="M69" s="105" t="n">
-        <v>5600747206098.197</v>
+        <v>12399289670375.54</v>
       </c>
       <c r="N69" s="105" t="n">
-        <v>5598406295068.483</v>
+        <v>12401869679656.08</v>
       </c>
       <c r="O69" s="105" t="n">
-        <v>5599492007344.488</v>
+        <v>12398694918426.65</v>
       </c>
       <c r="P69" s="105" t="n">
-        <v>5605100423907.044</v>
+        <v>12393156267034.1</v>
       </c>
       <c r="Q69" s="105" t="n">
-        <v>5616628623435.315</v>
+        <v>12389200498238.27</v>
       </c>
       <c r="R69" s="105" t="n">
-        <v>5634115037803.69</v>
+        <v>12389783983249.96</v>
       </c>
       <c r="S69" s="105" t="n">
-        <v>5656843688008.663</v>
+        <v>12384358573256.19</v>
       </c>
       <c r="T69" s="105" t="n">
-        <v>5683407504567.446</v>
+        <v>12384236871750.51</v>
       </c>
       <c r="U69" s="105" t="n">
-        <v>5713810071200.28</v>
+        <v>12380270751650.16</v>
       </c>
       <c r="V69" s="105" t="n">
-        <v>5748255829271.002</v>
+        <v>12381956784898.84</v>
       </c>
       <c r="W69" s="105" t="n">
-        <v>5785824615183.475</v>
+        <v>12386850222454.51</v>
       </c>
       <c r="X69" s="105" t="n">
-        <v>5824966340723.356</v>
+        <v>12394048463950.54</v>
       </c>
       <c r="Y69" s="105" t="n">
-        <v>5866349470695.697</v>
+        <v>12412315707459.15</v>
       </c>
       <c r="Z69" s="105" t="n">
-        <v>5909640586546.874</v>
+        <v>12433701004371.46</v>
       </c>
       <c r="AA69" s="105" t="n">
-        <v>5955031539964.684</v>
+        <v>12470315904003.53</v>
       </c>
       <c r="AB69" s="105" t="n">
-        <v>6001093330689.964</v>
+        <v>12513602856847.17</v>
       </c>
       <c r="AC69" s="105" t="n">
-        <v>6046949499924.616</v>
+        <v>12562843868836.27</v>
       </c>
       <c r="AD69" s="105" t="n">
-        <v>6092603862151.035</v>
+        <v>12616319862574.66</v>
       </c>
       <c r="AE69" s="105" t="n">
-        <v>6137772973971.312</v>
+        <v>12677031193267.34</v>
       </c>
       <c r="AF69" s="105" t="n">
-        <v>6179013639036.331</v>
+        <v>12710445902008.19</v>
       </c>
       <c r="AG69" s="105" t="n">
-        <v>6220058733766.902</v>
+        <v>12744775917882.45</v>
       </c>
       <c r="AH69" s="105" t="n">
-        <v>6261103328470.007</v>
+        <v>12784136119101.07</v>
       </c>
       <c r="AI69" s="105" t="n">
-        <v>6302047812652.647</v>
+        <v>12824372566900.59</v>
       </c>
       <c r="AJ69" s="105" t="n">
-        <v>6343233320329.742</v>
+        <v>12867464529510.51</v>
       </c>
       <c r="AK69" s="105" t="n">
-        <v>6384549485036.264</v>
+        <v>12907858061801.29</v>
       </c>
       <c r="AL69" s="105" t="n">
-        <v>6426340796625.944</v>
+        <v>12948994608893.87</v>
       </c>
       <c r="AM69" s="105" t="n">
-        <v>6468810151217.7</v>
+        <v>12991565062317.27</v>
       </c>
       <c r="AN69" s="105" t="n">
-        <v>6511856059248.271</v>
+        <v>13035621892310.35</v>
       </c>
       <c r="AO69" s="105" t="n">
-        <v>6555386791223.942</v>
+        <v>13081248382706.2</v>
       </c>
     </row>
     <row r="70">
@@ -55709,100 +55709,100 @@
         </is>
       </c>
       <c r="J71" s="105" t="n">
-        <v>4677426068126.383</v>
+        <v>18667168006683.53</v>
       </c>
       <c r="K71" s="105" t="n">
-        <v>4706776861570.607</v>
+        <v>18695968715525.66</v>
       </c>
       <c r="L71" s="105" t="n">
-        <v>4737671202733.28</v>
+        <v>18717137481398.64</v>
       </c>
       <c r="M71" s="105" t="n">
-        <v>4768339711286.029</v>
+        <v>18720902533868.2</v>
       </c>
       <c r="N71" s="105" t="n">
-        <v>4799689117354.299</v>
+        <v>18715786524369.62</v>
       </c>
       <c r="O71" s="105" t="n">
-        <v>4832586306344.273</v>
+        <v>18702873470745.46</v>
       </c>
       <c r="P71" s="105" t="n">
-        <v>4867186509688.716</v>
+        <v>18688253217554.69</v>
       </c>
       <c r="Q71" s="105" t="n">
-        <v>4904830448715.195</v>
+        <v>18683918993121.62</v>
       </c>
       <c r="R71" s="105" t="n">
-        <v>4944972209049.696</v>
+        <v>18697591096021.56</v>
       </c>
       <c r="S71" s="105" t="n">
-        <v>4985677875492.758</v>
+        <v>18708228710565.53</v>
       </c>
       <c r="T71" s="105" t="n">
-        <v>5026257806724.648</v>
+        <v>18736751264864.16</v>
       </c>
       <c r="U71" s="105" t="n">
-        <v>5066976732643.282</v>
+        <v>18766649854633.91</v>
       </c>
       <c r="V71" s="105" t="n">
-        <v>5107903101854.39</v>
+        <v>18812152904248.43</v>
       </c>
       <c r="W71" s="105" t="n">
-        <v>5148012116171.086</v>
+        <v>18868659186541.97</v>
       </c>
       <c r="X71" s="105" t="n">
-        <v>5186824095882.558</v>
+        <v>18930408004301.5</v>
       </c>
       <c r="Y71" s="105" t="n">
-        <v>5226852692920.118</v>
+        <v>19007834637853.85</v>
       </c>
       <c r="Z71" s="105" t="n">
-        <v>5267991989544.973</v>
+        <v>19082897594306.18</v>
       </c>
       <c r="AA71" s="105" t="n">
-        <v>5310643309608.936</v>
+        <v>19181145945891.28</v>
       </c>
       <c r="AB71" s="105" t="n">
-        <v>5353527878580.199</v>
+        <v>19285478360795.41</v>
       </c>
       <c r="AC71" s="105" t="n">
-        <v>5396226089639.264</v>
+        <v>19391332056528.59</v>
       </c>
       <c r="AD71" s="105" t="n">
-        <v>5438965256954.657</v>
+        <v>19501752804466.16</v>
       </c>
       <c r="AE71" s="105" t="n">
-        <v>5481322563318.974</v>
+        <v>19622346885675.79</v>
       </c>
       <c r="AF71" s="105" t="n">
-        <v>5516151776093.63</v>
+        <v>19676882159431.44</v>
       </c>
       <c r="AG71" s="105" t="n">
-        <v>5550692247240.815</v>
+        <v>19730593202782.43</v>
       </c>
       <c r="AH71" s="105" t="n">
-        <v>5585846853148.413</v>
+        <v>19795405999266.63</v>
       </c>
       <c r="AI71" s="105" t="n">
-        <v>5621431926352.611</v>
+        <v>19865887818852.77</v>
       </c>
       <c r="AJ71" s="105" t="n">
-        <v>5657817998865.653</v>
+        <v>19948844241507.9</v>
       </c>
       <c r="AK71" s="105" t="n">
-        <v>5694272013827.126</v>
+        <v>20030554469642.06</v>
       </c>
       <c r="AL71" s="105" t="n">
-        <v>5731144459314.646</v>
+        <v>20114732716289.79</v>
       </c>
       <c r="AM71" s="105" t="n">
-        <v>5768303503464.816</v>
+        <v>20198865917826.18</v>
       </c>
       <c r="AN71" s="105" t="n">
-        <v>5805854357286.008</v>
+        <v>20280181334149.91</v>
       </c>
       <c r="AO71" s="105" t="n">
-        <v>5843894153773.905</v>
+        <v>20356958489067.05</v>
       </c>
     </row>
     <row r="72">
@@ -55817,100 +55817,100 @@
         </is>
       </c>
       <c r="J72" s="105" t="n">
-        <v>39995213139.22304</v>
+        <v>1885075009059.26</v>
       </c>
       <c r="K72" s="105" t="n">
-        <v>39360450031.08216</v>
+        <v>1880531345739.29</v>
       </c>
       <c r="L72" s="105" t="n">
-        <v>38911604027.62592</v>
+        <v>1874495817812.658</v>
       </c>
       <c r="M72" s="105" t="n">
-        <v>38601766841.51191</v>
+        <v>1865899925218.335</v>
       </c>
       <c r="N72" s="105" t="n">
-        <v>38423846529.32891</v>
+        <v>1854673432086.505</v>
       </c>
       <c r="O72" s="105" t="n">
-        <v>38367579609.88773</v>
+        <v>1840209223273.595</v>
       </c>
       <c r="P72" s="105" t="n">
-        <v>38390065319.74011</v>
+        <v>1821735191064.329</v>
       </c>
       <c r="Q72" s="105" t="n">
-        <v>38485057777.51411</v>
+        <v>1799267285739.988</v>
       </c>
       <c r="R72" s="105" t="n">
-        <v>38639133938.62923</v>
+        <v>1771685368303.072</v>
       </c>
       <c r="S72" s="105" t="n">
-        <v>38811559468.93555</v>
+        <v>1735042102393.11</v>
       </c>
       <c r="T72" s="105" t="n">
-        <v>39005249341.98235</v>
+        <v>1690538280683.184</v>
       </c>
       <c r="U72" s="105" t="n">
-        <v>39201682734.73074</v>
+        <v>1635996731965.826</v>
       </c>
       <c r="V72" s="105" t="n">
-        <v>39407652324.50555</v>
+        <v>1573570974457.601</v>
       </c>
       <c r="W72" s="105" t="n">
-        <v>39622369700.19627</v>
+        <v>1504695913232.387</v>
       </c>
       <c r="X72" s="105" t="n">
-        <v>39820217483.1122</v>
+        <v>1429950482975.95</v>
       </c>
       <c r="Y72" s="105" t="n">
-        <v>40032743963.22569</v>
+        <v>1351000937980.449</v>
       </c>
       <c r="Z72" s="105" t="n">
-        <v>40240593944.95894</v>
+        <v>1267553439458.549</v>
       </c>
       <c r="AA72" s="105" t="n">
-        <v>40465666610.03648</v>
+        <v>1183226731384.256</v>
       </c>
       <c r="AB72" s="105" t="n">
-        <v>40690375012.06992</v>
+        <v>1097769705521.69</v>
       </c>
       <c r="AC72" s="105" t="n">
-        <v>40903153071.78458</v>
+        <v>1011429601972.372</v>
       </c>
       <c r="AD72" s="105" t="n">
-        <v>41123950581.063</v>
+        <v>925354884971.7411</v>
       </c>
       <c r="AE72" s="105" t="n">
-        <v>41340831626.0589</v>
+        <v>840443973845.4902</v>
       </c>
       <c r="AF72" s="105" t="n">
-        <v>41566348332.04147</v>
+        <v>753776982896.7524</v>
       </c>
       <c r="AG72" s="105" t="n">
-        <v>41778328719.46249</v>
+        <v>670086982558.8706</v>
       </c>
       <c r="AH72" s="105" t="n">
-        <v>42000709501.39207</v>
+        <v>590385943561.8242</v>
       </c>
       <c r="AI72" s="105" t="n">
-        <v>42222811493.07866</v>
+        <v>514945737921.9691</v>
       </c>
       <c r="AJ72" s="105" t="n">
-        <v>42456823284.1377</v>
+        <v>444694997950.7062</v>
       </c>
       <c r="AK72" s="105" t="n">
-        <v>42679281345.55836</v>
+        <v>380061253951.9631</v>
       </c>
       <c r="AL72" s="105" t="n">
-        <v>42901983931.68616</v>
+        <v>321904150642.8547</v>
       </c>
       <c r="AM72" s="105" t="n">
-        <v>43124761695.95419</v>
+        <v>270556368393.598</v>
       </c>
       <c r="AN72" s="105" t="n">
-        <v>43348112830.29434</v>
+        <v>225973113907.5413</v>
       </c>
       <c r="AO72" s="105" t="n">
-        <v>43572594899.27948</v>
+        <v>187885573767.6655</v>
       </c>
     </row>
     <row r="73">
@@ -56028,100 +56028,100 @@
         </is>
       </c>
       <c r="J74" s="105" t="n">
-        <v>979493591938.1503</v>
+        <v>3244976110777.311</v>
       </c>
       <c r="K74" s="105" t="n">
-        <v>988277077748.9257</v>
+        <v>3238623360739.912</v>
       </c>
       <c r="L74" s="105" t="n">
-        <v>997320947768.9496</v>
+        <v>3230514504966.11</v>
       </c>
       <c r="M74" s="105" t="n">
-        <v>1005612327681.814</v>
+        <v>3218996998152.323</v>
       </c>
       <c r="N74" s="105" t="n">
-        <v>1013725033940.548</v>
+        <v>3206132017618.063</v>
       </c>
       <c r="O74" s="105" t="n">
-        <v>1022197143328.455</v>
+        <v>3192288029430.012</v>
       </c>
       <c r="P74" s="105" t="n">
-        <v>1030287307631.494</v>
+        <v>3177043244213.917</v>
       </c>
       <c r="Q74" s="105" t="n">
-        <v>1038501559721.186</v>
+        <v>3162919027004.747</v>
       </c>
       <c r="R74" s="105" t="n">
-        <v>1047051194968.468</v>
+        <v>3150246048190.901</v>
       </c>
       <c r="S74" s="105" t="n">
-        <v>1054936876776.968</v>
+        <v>3135724732141.943</v>
       </c>
       <c r="T74" s="105" t="n">
-        <v>1062811967525.541</v>
+        <v>3122834888750.704</v>
       </c>
       <c r="U74" s="105" t="n">
-        <v>1070103927741.971</v>
+        <v>3108302798012.378</v>
       </c>
       <c r="V74" s="105" t="n">
-        <v>1077305640664.146</v>
+        <v>3095027481681.69</v>
       </c>
       <c r="W74" s="105" t="n">
-        <v>1084638341376.8</v>
+        <v>3084082154486.646</v>
       </c>
       <c r="X74" s="105" t="n">
-        <v>1091124517997.67</v>
+        <v>3073477116292.745</v>
       </c>
       <c r="Y74" s="105" t="n">
-        <v>1097910229004.195</v>
+        <v>3066364015314.106</v>
       </c>
       <c r="Z74" s="105" t="n">
-        <v>1104217544868.587</v>
+        <v>3061035554172.48</v>
       </c>
       <c r="AA74" s="105" t="n">
-        <v>1111000299695.488</v>
+        <v>3062080880498.556</v>
       </c>
       <c r="AB74" s="105" t="n">
-        <v>1117689729781.142</v>
+        <v>3067525933236.674</v>
       </c>
       <c r="AC74" s="105" t="n">
-        <v>1123828917784.96</v>
+        <v>3075474343076.671</v>
       </c>
       <c r="AD74" s="105" t="n">
-        <v>1130277584327.447</v>
+        <v>3086114832840.551</v>
       </c>
       <c r="AE74" s="105" t="n">
-        <v>1136546798726.759</v>
+        <v>3098815918821.968</v>
       </c>
       <c r="AF74" s="105" t="n">
-        <v>1142068496562.345</v>
+        <v>3107195108626.88</v>
       </c>
       <c r="AG74" s="105" t="n">
-        <v>1147023095506.877</v>
+        <v>3114256568145.978</v>
       </c>
       <c r="AH74" s="105" t="n">
-        <v>1152363692837.432</v>
+        <v>3121318628055.231</v>
       </c>
       <c r="AI74" s="105" t="n">
-        <v>1157633524186.334</v>
+        <v>3126237387141.899</v>
       </c>
       <c r="AJ74" s="105" t="n">
-        <v>1163328890475.104</v>
+        <v>3130274340273.38</v>
       </c>
       <c r="AK74" s="105" t="n">
-        <v>1168497977726.128</v>
+        <v>3131406094248.269</v>
       </c>
       <c r="AL74" s="105" t="n">
-        <v>1173627650162.878</v>
+        <v>3131835614437.762</v>
       </c>
       <c r="AM74" s="105" t="n">
-        <v>1178728084177.267</v>
+        <v>3132272033049.788</v>
       </c>
       <c r="AN74" s="105" t="n">
-        <v>1183810273394.304</v>
+        <v>3132758708546.386</v>
       </c>
       <c r="AO74" s="105" t="n">
-        <v>1188883283193.069</v>
+        <v>3133333943949.499</v>
       </c>
     </row>
     <row r="75">
@@ -56131,100 +56131,100 @@
         </is>
       </c>
       <c r="J75" s="93" t="n">
-        <v>37147313803.68789</v>
+        <v>254411916342.1003</v>
       </c>
       <c r="K75" s="93" t="n">
-        <v>37227003074.60125</v>
+        <v>254192532737.3963</v>
       </c>
       <c r="L75" s="93" t="n">
-        <v>37327011336.66843</v>
+        <v>253793369380.9022</v>
       </c>
       <c r="M75" s="93" t="n">
-        <v>37410990864.89785</v>
+        <v>253068275846.105</v>
       </c>
       <c r="N75" s="93" t="n">
-        <v>37499623870.92701</v>
+        <v>252044557706.0436</v>
       </c>
       <c r="O75" s="93" t="n">
-        <v>37614610698.50262</v>
+        <v>250617880797.5579</v>
       </c>
       <c r="P75" s="93" t="n">
-        <v>37719972782.45122</v>
+        <v>248611869496.0735</v>
       </c>
       <c r="Q75" s="93" t="n">
-        <v>37824803964.73115</v>
+        <v>246025042279.4339</v>
       </c>
       <c r="R75" s="93" t="n">
-        <v>37938553894.01634</v>
+        <v>242665862788.4396</v>
       </c>
       <c r="S75" s="93" t="n">
-        <v>38031812289.09374</v>
+        <v>238082750891.077</v>
       </c>
       <c r="T75" s="93" t="n">
-        <v>38129372220.42673</v>
+        <v>232451211176.7766</v>
       </c>
       <c r="U75" s="93" t="n">
-        <v>38209895106.64486</v>
+        <v>225499733658.1951</v>
       </c>
       <c r="V75" s="93" t="n">
-        <v>38289611206.64177</v>
+        <v>217531964553.3769</v>
       </c>
       <c r="W75" s="93" t="n">
-        <v>38379330923.5338</v>
+        <v>208788534069.8318</v>
       </c>
       <c r="X75" s="93" t="n">
-        <v>38447303572.60699</v>
+        <v>199274048366.9418</v>
       </c>
       <c r="Y75" s="93" t="n">
-        <v>38531555451.21155</v>
+        <v>189232887247.6469</v>
       </c>
       <c r="Z75" s="93" t="n">
-        <v>38603384752.6885</v>
+        <v>178618860731.6172</v>
       </c>
       <c r="AA75" s="93" t="n">
-        <v>38696065637.0929</v>
+        <v>167818921826.0599</v>
       </c>
       <c r="AB75" s="93" t="n">
-        <v>38788932649.92506</v>
+        <v>156815499158.362</v>
       </c>
       <c r="AC75" s="93" t="n">
-        <v>38865772147.15279</v>
+        <v>145642778938.195</v>
       </c>
       <c r="AD75" s="93" t="n">
-        <v>38957082419.34727</v>
+        <v>134496759883.9189</v>
       </c>
       <c r="AE75" s="93" t="n">
-        <v>39047841645.88869</v>
+        <v>123534703774.2169</v>
       </c>
       <c r="AF75" s="93" t="n">
-        <v>39237548205.2156</v>
+        <v>112737931885.0257</v>
       </c>
       <c r="AG75" s="93" t="n">
-        <v>39407771195.78817</v>
+        <v>102422975676.151</v>
       </c>
       <c r="AH75" s="93" t="n">
-        <v>39591255764.2121</v>
+        <v>92798250830.01904</v>
       </c>
       <c r="AI75" s="93" t="n">
-        <v>39772309056.732</v>
+        <v>83935367973.10646</v>
       </c>
       <c r="AJ75" s="93" t="n">
-        <v>39967982267.20461</v>
+        <v>75971316030.68185</v>
       </c>
       <c r="AK75" s="93" t="n">
-        <v>40145574338.7831</v>
+        <v>68913436801.98323</v>
       </c>
       <c r="AL75" s="93" t="n">
-        <v>40321812252.81348</v>
+        <v>62836119264.98311</v>
       </c>
       <c r="AM75" s="93" t="n">
-        <v>40497045635.14516</v>
+        <v>57740875734.95475</v>
       </c>
       <c r="AN75" s="93" t="n">
-        <v>40671652188.94797</v>
+        <v>53585212573.88683</v>
       </c>
       <c r="AO75" s="93" t="n">
-        <v>40845943369.48902</v>
+        <v>50295691576.21679</v>
       </c>
     </row>
     <row r="76">
@@ -56342,100 +56342,100 @@
         </is>
       </c>
       <c r="J77" s="105" t="n">
-        <v>757150004438.8478</v>
+        <v>1960613029607.729</v>
       </c>
       <c r="K77" s="105" t="n">
-        <v>756524680416.3566</v>
+        <v>1964229611361.154</v>
       </c>
       <c r="L77" s="105" t="n">
-        <v>757234500114.3206</v>
+        <v>1968593682823.075</v>
       </c>
       <c r="M77" s="105" t="n">
-        <v>758545072366.3927</v>
+        <v>1972533312555.802</v>
       </c>
       <c r="N77" s="105" t="n">
-        <v>760700568708.4513</v>
+        <v>1976828361214.747</v>
       </c>
       <c r="O77" s="105" t="n">
-        <v>763900446801.7708</v>
+        <v>1981574097887.933</v>
       </c>
       <c r="P77" s="105" t="n">
-        <v>767589559680.2734</v>
+        <v>1986367713485.89</v>
       </c>
       <c r="Q77" s="105" t="n">
-        <v>772004769829.3459</v>
+        <v>1992438823129.91</v>
       </c>
       <c r="R77" s="105" t="n">
-        <v>777134553689.2501</v>
+        <v>1999930218261.624</v>
       </c>
       <c r="S77" s="105" t="n">
-        <v>782221991736.3285</v>
+        <v>2006571593020.442</v>
       </c>
       <c r="T77" s="105" t="n">
-        <v>787512939186.4902</v>
+        <v>2014280918735.303</v>
       </c>
       <c r="U77" s="105" t="n">
-        <v>792624059704.7061</v>
+        <v>2021131473465.192</v>
       </c>
       <c r="V77" s="105" t="n">
-        <v>797790817974.8853</v>
+        <v>2028361487141.797</v>
       </c>
       <c r="W77" s="105" t="n">
-        <v>803061767334.2626</v>
+        <v>2036016132491.644</v>
       </c>
       <c r="X77" s="105" t="n">
-        <v>807826254596.5227</v>
+        <v>2042596978834.004</v>
       </c>
       <c r="Y77" s="105" t="n">
-        <v>812821778393.2052</v>
+        <v>2049454304967.457</v>
       </c>
       <c r="Z77" s="105" t="n">
-        <v>817590146782.1362</v>
+        <v>2054728041668.883</v>
       </c>
       <c r="AA77" s="105" t="n">
-        <v>822686624958.6903</v>
+        <v>2060736646513.604</v>
       </c>
       <c r="AB77" s="105" t="n">
-        <v>827731076145.1293</v>
+        <v>2065961414825.672</v>
       </c>
       <c r="AC77" s="105" t="n">
-        <v>832451541905.7045</v>
+        <v>2069781400444.234</v>
       </c>
       <c r="AD77" s="105" t="n">
-        <v>837345722686.3737</v>
+        <v>2073327369245.055</v>
       </c>
       <c r="AE77" s="105" t="n">
-        <v>842115649850.9669</v>
+        <v>2077171726017.124</v>
       </c>
       <c r="AF77" s="105" t="n">
-        <v>846505664665.7261</v>
+        <v>2077264821186.458</v>
       </c>
       <c r="AG77" s="105" t="n">
-        <v>850558430605.7987</v>
+        <v>2077146405020.238</v>
       </c>
       <c r="AH77" s="105" t="n">
-        <v>854850282079.7523</v>
+        <v>2078559554294.958</v>
       </c>
       <c r="AI77" s="105" t="n">
-        <v>859114743258.3586</v>
+        <v>2080951823312.656</v>
       </c>
       <c r="AJ77" s="105" t="n">
-        <v>863648800132.3809</v>
+        <v>2085291295104.358</v>
       </c>
       <c r="AK77" s="105" t="n">
-        <v>867884094811.3057</v>
+        <v>2089939835114.427</v>
       </c>
       <c r="AL77" s="105" t="n">
-        <v>872111425182.3267</v>
+        <v>2095506694015.66</v>
       </c>
       <c r="AM77" s="105" t="n">
-        <v>876332344212.5245</v>
+        <v>2101785573330.749</v>
       </c>
       <c r="AN77" s="105" t="n">
-        <v>880557282924.2366</v>
+        <v>2108475989810.64</v>
       </c>
       <c r="AO77" s="105" t="n">
-        <v>884795481366.4707</v>
+        <v>2115365926665.481</v>
       </c>
     </row>
     <row r="78">

</xml_diff>